<commit_message>
changes to the objects
</commit_message>
<xml_diff>
--- a/pkg/excels/output/О-01-00003.xlsx
+++ b/pkg/excels/output/О-01-00003.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>ОАО  "Таджикгидроэлектромонтаж"</t>
   </si>
@@ -236,13 +236,13 @@
 подпись зав. склада                                                                                                                                                                     </t>
   </si>
   <si>
-    <t>M-0004</t>
-  </si>
-  <si>
-    <t>Зубачистка</t>
-  </si>
-  <si>
-    <t>штук</t>
+    <t>о-0001</t>
+  </si>
+  <si>
+    <t>Вилка</t>
+  </si>
+  <si>
+    <t>шт</t>
   </si>
   <si>
     <t/>
@@ -317,7 +317,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="8"/>
       <color/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -530,7 +530,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -670,154 +670,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <themeElements>
-    <clrScheme name="Office">
-      <dk1>
-        <sysClr val="windowText" lastClr="000000"/>
-      </dk1>
-      <lt1>
-        <sysClr val="window" lastClr="FFFFFF"/>
-      </lt1>
-      <dk2>
-        <srgbClr val="44546A"/>
-      </dk2>
-      <lt2>
-        <srgbClr val="E7E6E6"/>
-      </lt2>
-      <accent1>
-        <srgbClr val="4472C4"/>
-      </accent1>
-      <accent2>
-        <srgbClr val="ED7D31"/>
-      </accent2>
-      <accent3>
-        <srgbClr val="A5A5A5"/>
-      </accent3>
-      <accent4>
-        <srgbClr val="FFC000"/>
-      </accent4>
-      <accent5>
-        <srgbClr val="5B9BD5"/>
-      </accent5>
-      <accent6>
-        <srgbClr val="70AD47"/>
-      </accent6>
-      <hlink>
-        <srgbClr val="0563C1"/>
-      </hlink>
-      <folHlink>
-        <srgbClr val="954F72"/>
-      </folHlink>
-    </clrScheme>
-    <fontScheme name="Office">
-      <majorFont>
-        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック Light"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线 Light"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Times New Roman"/>
-        <font script="Hebr" typeface="Times New Roman"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="MoolBoran"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Times New Roman"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </majorFont>
-      <minorFont>
-        <latin typeface="Calibri" panose="020F0502020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Arial"/>
-        <font script="Hebr" typeface="Arial"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="DaunPenh"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Arial"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </minorFont>
-    </fontScheme>
-    <fmtScheme name="Office">
-      <fillStyleLst>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -873,8 +873,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </fillStyleLst>
-      <lnStyleLst>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -896,8 +896,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </lnStyleLst>
-      <effectStyleLst>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -913,8 +913,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </effectStyleLst>
-      <bgFillStyleLst>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -951,17 +951,17 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </bgFillStyleLst>
-    </fmtScheme>
-  </themeElements>
-  <objectDefaults/>
-  <extraClrSchemeLst/>
-  <extLst>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </extLst>
-</theme>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -988,24 +988,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="50.45" customHeight="true">
-      <c r="A1" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36">
-        <v>5</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>28</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
@@ -1073,134 +1069,182 @@
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="5"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+    <row r="5">
+      <c r="A5" s="36">
+        <v>1</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="36">
+        <v>10</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="36">
+        <v>2</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="36">
+        <v>10</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="34" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="7" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34" t="s">
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18.6" customHeight="true">
-      <c r="A8" s="3"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="34"/>
-    </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="18.6" customHeight="true">
       <c r="A9" s="3"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="20"/>
       <c r="H9" s="11"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="22"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="32" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="7" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34" t="s">
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="35"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="H13" s="7" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" s="3"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13"/>
+    <row r="14" spans="1:11">
+      <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34" t="s">
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="37"/>
+    <row r="15" spans="1:11">
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:K11"/>
+  <mergeCells count="22">
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:K12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="I4:K4"/>
@@ -1210,6 +1254,10 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E3:H3"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup r:id="rId1" orientation="portrait" paperSize="9" verticalDpi="0"/>

</xml_diff>